<commit_message>
Update Std von Peric
</commit_message>
<xml_diff>
--- a/Dokumente/Stundenaufzeichnung.xlsx
+++ b/Dokumente/Stundenaufzeichnung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68157115d40ac8e2/Desktop/School/Thesis/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68157115d40ac8e2/Desktop/School/Thesis/AberGymMobile/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="417" documentId="11_AD4DB114E441178AC67DF45DD616F01C683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD48FE14-5735-4B62-950E-C27416F36F46}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="11_AD4DB114E441178AC67DF45DD616F01C683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B2970F5-1498-469D-B3C3-8EE75A29BE13}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Erfassungszeitraum</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Gesamt Stundenanzahl vom Projekt</t>
+  </si>
+  <si>
+    <t>Teil                   (Prog,Prot)</t>
+  </si>
+  <si>
+    <t>Prot</t>
+  </si>
+  <si>
+    <t>Stundenaufzeichnung erstellen</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1176,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1220,6 +1229,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="80" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="74" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="75" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="76" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="79" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="71" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1238,6 +1270,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="72" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="73" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1247,17 +1285,134 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="77" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="78" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="63" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="64" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="59" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1277,161 +1432,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="63" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="64" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="59" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="71" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="72" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="73" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="74" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="75" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="76" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="77" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="78" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="79" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="80" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -1718,7 +1742,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,31 +1751,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="90"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94">
+      <c r="A2" s="32">
         <f>Projektstundennachweis!I50+Projektstundennachweis!R50</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
@@ -1765,17 +1789,17 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="93"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:9" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
@@ -1789,11 +1813,11 @@
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="20" t="s">
         <v>12</v>
       </c>
@@ -1804,34 +1828,35 @@
       <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="84">
-        <v>0</v>
-      </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="85"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="84">
-        <v>0</v>
-      </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="33">
+        <f>Projektstundennachweis!I10</f>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
@@ -1845,11 +1870,11 @@
       <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="20" t="s">
         <v>13</v>
       </c>
@@ -1860,34 +1885,34 @@
       <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="84">
-        <v>0</v>
-      </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="85"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="86">
-        <v>0</v>
-      </c>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="87"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41">
+        <v>0</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1918,269 +1943,278 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E1358-462B-47CB-9766-E4587C35E91E}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:F42"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="75" t="s">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="52"/>
+      <c r="L1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="77"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="61"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="32" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="79" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="80"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="58"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="26" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="81"/>
-      <c r="L3" s="82" t="s">
+      <c r="K3" s="54"/>
+      <c r="L3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="83"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="56"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="59"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="82"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="89"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="84"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="77"/>
+      <c r="L5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="M5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="66" t="s">
+      <c r="N5" s="89"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="67"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="39"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="68"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="85"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="69" t="s">
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="71" t="s">
+      <c r="I6" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="62"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="69" t="s">
+      <c r="J6" s="78"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="92"/>
+      <c r="P6" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="69" t="s">
+      <c r="Q6" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="71" t="s">
+      <c r="R6" s="65" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="71"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="65"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="71"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="92"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="65"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="72"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="66"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="101"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.75347222222222221</v>
+      </c>
       <c r="I10" s="7">
         <f>H10-G10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="58"/>
-      <c r="K10" s="53"/>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="95"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="7">
@@ -2189,24 +2223,24 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="64"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="7">
         <f>H11-G11</f>
         <v>0</v>
       </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="35"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="63"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="36"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="64"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="7">
@@ -2215,24 +2249,24 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="7">
         <f t="shared" ref="I12:I49" si="0">H12-G12</f>
         <v>0</v>
       </c>
-      <c r="J12" s="55"/>
-      <c r="K12" s="35"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="36"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="64"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="7">
@@ -2241,24 +2275,24 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="35"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="63"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="36"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="64"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="7">
@@ -2267,24 +2301,24 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="55"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="63"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="36"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="64"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="7">
@@ -2293,24 +2327,24 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="55"/>
-      <c r="K15" s="35"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="63"/>
       <c r="L15" s="10"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="36"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="64"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="7">
@@ -2319,24 +2353,24 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="55"/>
-      <c r="K16" s="35"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="63"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="36"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="64"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="7">
@@ -2345,24 +2379,24 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J17" s="55"/>
-      <c r="K17" s="35"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="63"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="36"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="64"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="7">
@@ -2371,24 +2405,24 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="64"/>
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
       <c r="I18" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="35"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="63"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="36"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="64"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="7">
@@ -2397,24 +2431,24 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
       <c r="G19" s="2"/>
       <c r="H19" s="3"/>
       <c r="I19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="55"/>
-      <c r="K19" s="35"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="63"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="36"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="64"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="7">
@@ -2423,24 +2457,24 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="2"/>
       <c r="H20" s="3"/>
       <c r="I20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="55"/>
-      <c r="K20" s="35"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="63"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="36"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="64"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="7">
@@ -2449,24 +2483,24 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="2"/>
       <c r="H21" s="3"/>
       <c r="I21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="55"/>
-      <c r="K21" s="35"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="63"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="36"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="64"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="7">
@@ -2475,24 +2509,24 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
       <c r="G22" s="2"/>
       <c r="H22" s="3"/>
       <c r="I22" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="55"/>
-      <c r="K22" s="35"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="63"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="36"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="64"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="7">
@@ -2501,24 +2535,24 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
       <c r="G23" s="2"/>
       <c r="H23" s="3"/>
       <c r="I23" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="55"/>
-      <c r="K23" s="35"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="36"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="64"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="7">
@@ -2527,24 +2561,24 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="64"/>
       <c r="G24" s="2"/>
       <c r="H24" s="3"/>
       <c r="I24" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="55"/>
-      <c r="K24" s="35"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="63"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="36"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="64"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="7">
@@ -2553,24 +2587,24 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="2"/>
       <c r="H25" s="3"/>
       <c r="I25" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="55"/>
-      <c r="K25" s="35"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63"/>
       <c r="L25" s="10"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="36"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="64"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="7">
@@ -2579,24 +2613,24 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
       <c r="G26" s="2"/>
       <c r="H26" s="3"/>
       <c r="I26" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="55"/>
-      <c r="K26" s="35"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="63"/>
       <c r="L26" s="10"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="36"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="64"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="7">
@@ -2605,24 +2639,24 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
       <c r="G27" s="2"/>
       <c r="H27" s="3"/>
       <c r="I27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J27" s="55"/>
-      <c r="K27" s="35"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
       <c r="L27" s="10"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="36"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="64"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="7">
@@ -2631,24 +2665,24 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
       <c r="G28" s="2"/>
       <c r="H28" s="3"/>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="55"/>
-      <c r="K28" s="35"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="36"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="64"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="7">
@@ -2657,24 +2691,24 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="2"/>
       <c r="H29" s="3"/>
       <c r="I29" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="55"/>
-      <c r="K29" s="35"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="63"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="36"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="64"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="7">
@@ -2683,24 +2717,24 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="63"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="64"/>
       <c r="G30" s="2"/>
       <c r="H30" s="3"/>
       <c r="I30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="55"/>
-      <c r="K30" s="35"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="63"/>
       <c r="L30" s="10"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="36"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="64"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="7">
@@ -2709,24 +2743,24 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="35"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
       <c r="G31" s="2"/>
       <c r="H31" s="3"/>
       <c r="I31" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="55"/>
-      <c r="K31" s="35"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="63"/>
       <c r="L31" s="10"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="36"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="64"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="7">
@@ -2735,24 +2769,24 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="35"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="64"/>
       <c r="G32" s="2"/>
       <c r="H32" s="3"/>
       <c r="I32" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="55"/>
-      <c r="K32" s="35"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="63"/>
       <c r="L32" s="10"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="36"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="64"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="7">
@@ -2761,24 +2795,24 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="35"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="63"/>
       <c r="C33" s="10"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="64"/>
       <c r="G33" s="2"/>
       <c r="H33" s="3"/>
       <c r="I33" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="55"/>
-      <c r="K33" s="35"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="63"/>
       <c r="L33" s="10"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="36"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="64"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="7">
@@ -2787,24 +2821,24 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="35"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="10"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
       <c r="G34" s="2"/>
       <c r="H34" s="3"/>
       <c r="I34" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J34" s="55"/>
-      <c r="K34" s="35"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="63"/>
       <c r="L34" s="10"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="36"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="64"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="7">
@@ -2813,24 +2847,24 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="35"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="64"/>
       <c r="G35" s="2"/>
       <c r="H35" s="3"/>
       <c r="I35" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="55"/>
-      <c r="K35" s="35"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63"/>
       <c r="L35" s="10"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="36"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="64"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="7">
@@ -2839,24 +2873,24 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
-      <c r="B36" s="35"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="63"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="2"/>
       <c r="H36" s="3"/>
       <c r="I36" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="55"/>
-      <c r="K36" s="35"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="63"/>
       <c r="L36" s="10"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="36"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="63"/>
+      <c r="O36" s="64"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="7">
@@ -2865,24 +2899,24 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="2"/>
       <c r="H37" s="3"/>
       <c r="I37" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J37" s="55"/>
-      <c r="K37" s="35"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="63"/>
       <c r="L37" s="10"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="36"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="64"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="7">
@@ -2891,50 +2925,50 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="57"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="74"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="97"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
       <c r="I38" s="7">
         <f>H38-G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="56"/>
-      <c r="K38" s="57"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="74"/>
       <c r="L38" s="10"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="96"/>
-      <c r="Q38" s="97"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="28"/>
       <c r="R38" s="7">
         <f>Q38-P38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="62"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="64"/>
       <c r="G39" s="2"/>
       <c r="H39" s="3"/>
       <c r="I39" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="55"/>
-      <c r="K39" s="35"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="63"/>
       <c r="L39" s="10"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="36"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="64"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="7">
@@ -2943,24 +2977,24 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
-      <c r="B40" s="35"/>
+      <c r="A40" s="62"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="64"/>
       <c r="G40" s="2"/>
       <c r="H40" s="3"/>
       <c r="I40" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="55"/>
-      <c r="K40" s="35"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="63"/>
       <c r="L40" s="10"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="36"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="63"/>
+      <c r="O40" s="64"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="7">
@@ -2969,24 +3003,24 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
-      <c r="B41" s="35"/>
+      <c r="A41" s="62"/>
+      <c r="B41" s="63"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="64"/>
       <c r="G41" s="2"/>
       <c r="H41" s="3"/>
       <c r="I41" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="55"/>
-      <c r="K41" s="35"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="63"/>
       <c r="L41" s="10"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="36"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="64"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="7">
@@ -2995,24 +3029,24 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="55"/>
-      <c r="B42" s="35"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="63"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="64"/>
       <c r="G42" s="2"/>
       <c r="H42" s="3"/>
       <c r="I42" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="55"/>
-      <c r="K42" s="35"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="63"/>
       <c r="L42" s="10"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="36"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="64"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="7">
@@ -3021,24 +3055,24 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="55"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="63"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="64"/>
       <c r="G43" s="2"/>
       <c r="H43" s="3"/>
       <c r="I43" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J43" s="55"/>
-      <c r="K43" s="35"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="63"/>
       <c r="L43" s="10"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="36"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="64"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="7">
@@ -3047,24 +3081,24 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="62"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="10"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="64"/>
       <c r="G44" s="2"/>
       <c r="H44" s="3"/>
       <c r="I44" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="55"/>
-      <c r="K44" s="35"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="63"/>
       <c r="L44" s="10"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="36"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="64"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="7">
@@ -3073,24 +3107,24 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="63"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="64"/>
       <c r="G45" s="2"/>
       <c r="H45" s="3"/>
       <c r="I45" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="55"/>
-      <c r="K45" s="35"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="63"/>
       <c r="L45" s="10"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="36"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="64"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="7">
@@ -3099,24 +3133,24 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="62"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="64"/>
       <c r="G46" s="2"/>
       <c r="H46" s="3"/>
       <c r="I46" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J46" s="55"/>
-      <c r="K46" s="35"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="63"/>
       <c r="L46" s="10"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="36"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="64"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="7">
@@ -3125,24 +3159,24 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="55"/>
-      <c r="B47" s="35"/>
+      <c r="A47" s="62"/>
+      <c r="B47" s="63"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="64"/>
       <c r="G47" s="2"/>
       <c r="H47" s="3"/>
       <c r="I47" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J47" s="55"/>
-      <c r="K47" s="35"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="63"/>
       <c r="L47" s="10"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="35"/>
-      <c r="O47" s="36"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="64"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="7">
@@ -3151,24 +3185,24 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="55"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="62"/>
+      <c r="B48" s="63"/>
       <c r="C48" s="10"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="64"/>
       <c r="G48" s="2"/>
       <c r="H48" s="3"/>
       <c r="I48" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J48" s="55"/>
-      <c r="K48" s="35"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="63"/>
       <c r="L48" s="10"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="35"/>
-      <c r="O48" s="36"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="64"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="7">
@@ -3177,24 +3211,24 @@
       </c>
     </row>
     <row r="49" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
-      <c r="B49" s="49"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="11"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="64"/>
       <c r="G49" s="4"/>
       <c r="H49" s="6"/>
       <c r="I49" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J49" s="48"/>
-      <c r="K49" s="49"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="68"/>
       <c r="L49" s="11"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="36"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="64"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="6"/>
       <c r="R49" s="8">
@@ -3203,31 +3237,31 @@
       </c>
     </row>
     <row r="50" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="50"/>
-      <c r="B50" s="51"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="12"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="52" t="s">
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="97"/>
+      <c r="G50" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="51"/>
-      <c r="I50" s="95">
+      <c r="H50" s="70"/>
+      <c r="I50" s="26">
         <f>SUM(I10:I49)</f>
-        <v>0</v>
-      </c>
-      <c r="J50" s="50"/>
-      <c r="K50" s="51"/>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="J50" s="69"/>
+      <c r="K50" s="70"/>
       <c r="L50" s="12"/>
-      <c r="M50" s="37"/>
-      <c r="N50" s="37"/>
-      <c r="O50" s="38"/>
-      <c r="P50" s="52" t="s">
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="97"/>
+      <c r="P50" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="Q50" s="51"/>
-      <c r="R50" s="95">
+      <c r="Q50" s="70"/>
+      <c r="R50" s="26">
         <f>SUM(R10:R49)</f>
         <v>0</v>
       </c>
@@ -3235,36 +3269,146 @@
     <row r="51" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="194">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D5:F9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="J4:R4"/>
+    <mergeCell ref="J5:K9"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:P9"/>
+    <mergeCell ref="Q6:Q9"/>
+    <mergeCell ref="R6:R9"/>
+    <mergeCell ref="L5:L9"/>
+    <mergeCell ref="M5:O9"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:R3"/>
+    <mergeCell ref="A5:B9"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
@@ -3289,146 +3433,36 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:R3"/>
-    <mergeCell ref="A5:B9"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="J4:R4"/>
-    <mergeCell ref="J5:K9"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:P9"/>
-    <mergeCell ref="Q6:Q9"/>
-    <mergeCell ref="R6:R9"/>
-    <mergeCell ref="L5:L9"/>
-    <mergeCell ref="M5:O9"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D5:F9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>